<commit_message>
Before Improving Apparatus Sequence
</commit_message>
<xml_diff>
--- a/Nature_NETS_NYPS_68Bus_IBR_all.xlsx
+++ b/Nature_NETS_NYPS_68Bus_IBR_all.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\Power-Communication-Isomorphism\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF5586F1-6A29-4AA5-91A5-0133A0DE722A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFD7F5B6-AFBC-40BC-B6E2-398769E0DE78}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10395" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bus" sheetId="1" r:id="rId1"/>
@@ -3290,7 +3290,7 @@
   <dimension ref="A1:J70"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="I3" sqref="I3:I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
@@ -3339,14 +3339,14 @@
         <v>0.05</v>
       </c>
       <c r="F3" s="2">
-        <f>E3/5</f>
+        <f t="shared" ref="F3:F18" si="0">E3/5</f>
         <v>0.01</v>
       </c>
       <c r="H3">
         <v>5</v>
       </c>
       <c r="I3">
-        <v>100000000</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.4">
@@ -3361,14 +3361,14 @@
         <v>0.05</v>
       </c>
       <c r="F4" s="2">
-        <f>E4/5</f>
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
       <c r="H4">
         <v>5</v>
       </c>
       <c r="I4">
-        <v>100000000</v>
+        <v>10000000</v>
       </c>
       <c r="J4" s="2"/>
     </row>
@@ -3384,14 +3384,14 @@
         <v>0.05</v>
       </c>
       <c r="F5" s="2">
-        <f>E5/5</f>
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
       <c r="H5">
         <v>5</v>
       </c>
       <c r="I5">
-        <v>100000000</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.4">
@@ -3406,14 +3406,14 @@
         <v>0.05</v>
       </c>
       <c r="F6" s="2">
-        <f>E6/5</f>
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
       <c r="H6">
         <v>5</v>
       </c>
       <c r="I6">
-        <v>100000000</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.4">
@@ -3428,14 +3428,14 @@
         <v>0.05</v>
       </c>
       <c r="F7" s="2">
-        <f>E7/5</f>
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
       <c r="H7">
         <v>5</v>
       </c>
       <c r="I7">
-        <v>100000000</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.4">
@@ -3450,14 +3450,14 @@
         <v>0.05</v>
       </c>
       <c r="F8" s="2">
-        <f>E8/5</f>
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
       <c r="H8">
         <v>5</v>
       </c>
       <c r="I8">
-        <v>100000000</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.4">
@@ -3472,14 +3472,14 @@
         <v>0.05</v>
       </c>
       <c r="F9" s="2">
-        <f>E9/5</f>
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
       <c r="H9">
         <v>5</v>
       </c>
       <c r="I9">
-        <v>100000000</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.4">
@@ -3494,14 +3494,14 @@
         <v>0.05</v>
       </c>
       <c r="F10" s="2">
-        <f>E10/5</f>
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
       <c r="H10">
         <v>5</v>
       </c>
       <c r="I10">
-        <v>100000000</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.4">
@@ -3516,14 +3516,14 @@
         <v>0.05</v>
       </c>
       <c r="F11" s="2">
-        <f>E11/5</f>
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
       <c r="H11">
         <v>5</v>
       </c>
       <c r="I11">
-        <v>100000000</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.4">
@@ -3538,14 +3538,14 @@
         <v>0.05</v>
       </c>
       <c r="F12" s="2">
-        <f>E12/5</f>
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
       <c r="H12">
         <v>5</v>
       </c>
       <c r="I12">
-        <v>100000000</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.4">
@@ -3560,14 +3560,14 @@
         <v>0.05</v>
       </c>
       <c r="F13" s="2">
-        <f>E13/5</f>
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
       <c r="H13">
         <v>5</v>
       </c>
       <c r="I13">
-        <v>100000000</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.4">
@@ -3582,14 +3582,14 @@
         <v>0.05</v>
       </c>
       <c r="F14" s="2">
-        <f>E14/5</f>
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
       <c r="H14">
         <v>5</v>
       </c>
       <c r="I14">
-        <v>100000000</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.4">
@@ -3604,14 +3604,14 @@
         <v>0.05</v>
       </c>
       <c r="F15" s="2">
-        <f>E15/5</f>
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
       <c r="H15">
         <v>5</v>
       </c>
       <c r="I15">
-        <v>100000000</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.4">
@@ -3626,14 +3626,14 @@
         <v>0.05</v>
       </c>
       <c r="F16" s="2">
-        <f>E16/5</f>
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
       <c r="H16">
         <v>5</v>
       </c>
       <c r="I16">
-        <v>100000000</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.4">
@@ -3648,14 +3648,14 @@
         <v>0.05</v>
       </c>
       <c r="F17" s="2">
-        <f>E17/5</f>
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
       <c r="H17">
         <v>5</v>
       </c>
       <c r="I17">
-        <v>100000000</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.4">
@@ -3670,14 +3670,14 @@
         <v>0.05</v>
       </c>
       <c r="F18" s="2">
-        <f>E18/5</f>
+        <f t="shared" si="0"/>
         <v>0.01</v>
       </c>
       <c r="H18">
         <v>5</v>
       </c>
       <c r="I18">
-        <v>100000000</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.4">

</xml_diff>